<commit_message>
update with sneaky solve and options files
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_dors_2.xlsx
+++ b/examples/Abatement/Data/techdata_dors_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="inputdisp" sheetId="1" r:id="rId1"/>
@@ -437,9 +437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G3" sqref="G3"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,9 +515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>0.01</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>0.02</v>
       </c>
       <c r="G3">
-        <v>6.5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ad hoc adjustment in EOP part
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_dors_2.xlsx
+++ b/examples/Abatement/Data/techdata_dors_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="inputdisp" sheetId="1" r:id="rId1"/>
@@ -437,9 +437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3"/>
+      <selection pane="topRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G2" sqref="G2"/>
     </sheetView>

</xml_diff>